<commit_message>
reduce protocol splitting complexity of assay.xlsx reader
</commit_message>
<xml_diff>
--- a/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTestFile.xlsx
+++ b/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTestFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\ISADotNet\tests\ISADotNet.Tests\ISADotNet.XLSX\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B79C9B-EC72-4E8D-84E8-71BB5522545B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A846DF-27C1-4815-AD84-C145ACE490B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44880" yWindow="4230" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GreatAssay" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="82">
   <si>
     <t>ASSAY METADATA</t>
   </si>
@@ -102,39 +102,6 @@
     <t>Parameter [temperature unit]</t>
   </si>
   <si>
-    <t>Term Source REF [temperature unit] (#h; #tUO:0000005)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [temperature unit] (#h; #tUO:0000005)</t>
-  </si>
-  <si>
-    <t>Unit [degree Celsius] (#h; #tUO:0000027; #u)</t>
-  </si>
-  <si>
-    <t>Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)</t>
-  </si>
-  <si>
-    <t>Factor [time]</t>
-  </si>
-  <si>
-    <t>Term Source REF [time] (#h; #tPATO:0000165)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [time] (#h; #tPATO:0000165)</t>
-  </si>
-  <si>
-    <t>Unit [hour] (#h; #tUO:0000032; #u)</t>
-  </si>
-  <si>
-    <t>Term Source REF [hour] (#h; #tUO:0000032; #u)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [hour] (#h; #tUO:0000032; #u)</t>
-  </si>
-  <si>
     <t>Weil</t>
   </si>
   <si>
@@ -186,78 +153,27 @@
     <t>UO</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000005</t>
-  </si>
-  <si>
     <t>degree Celsius</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/UO_0000027</t>
   </si>
   <si>
-    <t>PATO</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/PATO_0000165</t>
-  </si>
-  <si>
     <t>hour</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/UO_0000032</t>
   </si>
   <si>
-    <t>Parameter [time]</t>
-  </si>
-  <si>
-    <t>Term Source REF [time] (#h; #tEFO:0000721)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [time] (#h; #tEFO:0000721)</t>
-  </si>
-  <si>
-    <t>Unit [hour] (#2; #h; #tUO:0000032; #u)</t>
-  </si>
-  <si>
-    <t>Term Source REF [hour] (#2; #h; #tUO:0000032; #u)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [hour] (#2; #h; #tUO:0000032; #u)</t>
-  </si>
-  <si>
-    <t>Parameter [temperature]</t>
-  </si>
-  <si>
-    <t>Term Source REF [temperature] (#h; #tNCRO:0000029)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [temperature] (#h; #tNCRO:0000029)</t>
-  </si>
-  <si>
-    <t>Unit [degree Celsius] (#h; #tdegreeCelsius; #u)</t>
-  </si>
-  <si>
-    <t>Term Source REF [degree Celsius] (#h; #tdegreeCelsius; #u)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [degree Celsius] (#h; #tdegreeCelsius; #u)</t>
-  </si>
-  <si>
     <t>Trypsin/P</t>
   </si>
   <si>
     <t>Parameter [Peptidase]</t>
   </si>
   <si>
-    <t>Term Source REF [Peptidase] (#h; #tNCIT:C16965)</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/MS_1001313</t>
   </si>
   <si>
-    <t>Term Accession Number [Peptidase] (#h; #tNCIT:C16965)</t>
-  </si>
-  <si>
     <t>peptide_digestion</t>
   </si>
   <si>
@@ -273,21 +189,6 @@
     <t>Characteristics [leaf size]</t>
   </si>
   <si>
-    <t>Term Source REF [leaf size] (#h; #tTO:0002637)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [leaf size] (#h; #tTO:0002637)</t>
-  </si>
-  <si>
-    <t>Unit [square centimeter] (#h; #tUO:0000081; #u)</t>
-  </si>
-  <si>
-    <t>Term Source REF [square centimeter] (#h; #tUO:0000081; #u)</t>
-  </si>
-  <si>
-    <t>Term Accession Number [square centimeter] (#h; #tUO:0000081; #u)</t>
-  </si>
-  <si>
     <t>Leil</t>
   </si>
   <si>
@@ -295,6 +196,78 @@
   </si>
   <si>
     <t>SecondAssay</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Term Source REF (UO:0000005)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (UO:0000005)</t>
+  </si>
+  <si>
+    <t>Term Source REF (NCIT:C16965)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (NCIT:C16965)</t>
+  </si>
+  <si>
+    <t>Unit (#2)</t>
+  </si>
+  <si>
+    <t>Parameter [temperature#2]</t>
+  </si>
+  <si>
+    <t>Term Source REF (NCRO:0000029#2)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (NCRO:0000029#2)</t>
+  </si>
+  <si>
+    <t>Unit (#3)</t>
+  </si>
+  <si>
+    <t>Term Source REF (EFO:0000721#3)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (EFO:0000721#3)</t>
+  </si>
+  <si>
+    <t>Parameter [time#3]</t>
+  </si>
+  <si>
+    <t>Unit (#4)</t>
+  </si>
+  <si>
+    <t>Factor [time#4]</t>
+  </si>
+  <si>
+    <t>Term Source REF (PATO:0000165#4)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (PATO:0000165#4)</t>
+  </si>
+  <si>
+    <t>Term Source REF (TO:0002637)</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000081</t>
+  </si>
+  <si>
+    <t>Term Accession Number (TO:0002637)</t>
+  </si>
+  <si>
+    <t>square centimeter</t>
+  </si>
+  <si>
+    <t>Term Source REF (UO:0000005#2)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (UO:0000005#2)</t>
+  </si>
+  <si>
+    <t>Parameter [temperature unit#2]</t>
   </si>
 </sst>
 </file>
@@ -306,7 +279,7 @@
     <numFmt numFmtId="165" formatCode="0.00\ &quot;hour&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00\ &quot;square centimeter&quot;"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -451,6 +424,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -788,7 +769,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -831,8 +812,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -853,8 +835,9 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -888,6 +871,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -919,37 +903,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D5592EB8-A35A-47FA-8237-E24647011A72}" name="annotationTable" displayName="annotationTable" ref="A2:AC5" totalsRowShown="0">
-  <autoFilter ref="A2:AC5" xr:uid="{88500CAB-F747-471B-9764-53874357314F}"/>
-  <tableColumns count="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D5592EB8-A35A-47FA-8237-E24647011A72}" name="annotationTable" displayName="annotationTable" ref="A2:U5" totalsRowShown="0">
+  <autoFilter ref="A2:U5" xr:uid="{88500CAB-F747-471B-9764-53874357314F}"/>
+  <tableColumns count="21">
     <tableColumn id="1" xr3:uid="{05ADECE3-F51A-4AFF-93A3-A272607FC2A1}" name="Source Name"/>
     <tableColumn id="3" xr3:uid="{F907451C-B0DF-4F7B-86F9-144DE1FE40BD}" name="Parameter [temperature unit]" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{A4500BED-D244-441C-83E2-6D9D222F14BD}" name="Term Source REF [temperature unit] (#h; #tUO:0000005)"/>
-    <tableColumn id="5" xr3:uid="{9D1124C1-E0D6-41E1-838D-C39DA7AB8F7B}" name="Term Accession Number [temperature unit] (#h; #tUO:0000005)"/>
-    <tableColumn id="6" xr3:uid="{33FE2BA2-4B61-4AD3-B521-DD4F65B0BB63}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)"/>
-    <tableColumn id="7" xr3:uid="{A2DBF8A1-CC58-4ECC-BCC5-51571CA0B60C}" name="Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)"/>
-    <tableColumn id="8" xr3:uid="{B3B81C65-EED1-413B-8BDA-DCC53CBF37AB}" name="Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)"/>
+    <tableColumn id="6" xr3:uid="{33FE2BA2-4B61-4AD3-B521-DD4F65B0BB63}" name="Unit"/>
+    <tableColumn id="7" xr3:uid="{A2DBF8A1-CC58-4ECC-BCC5-51571CA0B60C}" name="Term Source REF (UO:0000005)"/>
+    <tableColumn id="8" xr3:uid="{B3B81C65-EED1-413B-8BDA-DCC53CBF37AB}" name="Term Accession Number (UO:0000005)"/>
     <tableColumn id="27" xr3:uid="{EF413547-19AF-42F1-9E31-6F48D00B75CF}" name="Parameter [Peptidase]"/>
-    <tableColumn id="28" xr3:uid="{AAD82B6E-D534-4041-A45F-3B4DE315F57C}" name="Term Source REF [Peptidase] (#h; #tNCIT:C16965)"/>
-    <tableColumn id="29" xr3:uid="{0832B850-0B29-42BE-8818-06D777F94D14}" name="Term Accession Number [Peptidase] (#h; #tNCIT:C16965)"/>
-    <tableColumn id="21" xr3:uid="{E885C835-8F07-49F7-8754-56F33C22EDA3}" name="Parameter [temperature]"/>
-    <tableColumn id="22" xr3:uid="{2D49AE9F-4297-4B6C-8D15-9DCC8ED4D6CB}" name="Term Source REF [temperature] (#h; #tNCRO:0000029)"/>
-    <tableColumn id="23" xr3:uid="{17E48AA3-FD59-499B-9487-1636C4EE20C6}" name="Term Accession Number [temperature] (#h; #tNCRO:0000029)"/>
-    <tableColumn id="24" xr3:uid="{BBE00F76-3C9D-4912-9F00-79E953EFA580}" name="Unit [degree Celsius] (#h; #tdegreeCelsius; #u)"/>
-    <tableColumn id="25" xr3:uid="{4AFB1872-5F15-4214-A991-0EDD612D46C7}" name="Term Source REF [degree Celsius] (#h; #tdegreeCelsius; #u)"/>
-    <tableColumn id="26" xr3:uid="{3E7927AE-9C04-424E-9AF3-067EB934366D}" name="Term Accession Number [degree Celsius] (#h; #tdegreeCelsius; #u)"/>
-    <tableColumn id="15" xr3:uid="{0C97A092-0954-4712-ADFD-111FF359043F}" name="Parameter [time]"/>
-    <tableColumn id="16" xr3:uid="{BE2F9C5A-3DB7-4B51-9114-2D93B4DEEE89}" name="Term Source REF [time] (#h; #tEFO:0000721)"/>
-    <tableColumn id="17" xr3:uid="{8B51B781-39E4-4112-8F04-4DFEC03CA9FF}" name="Term Accession Number [time] (#h; #tEFO:0000721)"/>
-    <tableColumn id="18" xr3:uid="{48EE2CE6-DE17-43D9-931B-B49173F44C6D}" name="Unit [hour] (#2; #h; #tUO:0000032; #u)"/>
-    <tableColumn id="19" xr3:uid="{6792D8C2-693B-4BC9-883A-51034FF96CE1}" name="Term Source REF [hour] (#2; #h; #tUO:0000032; #u)"/>
-    <tableColumn id="20" xr3:uid="{44AC5DB4-A15D-4ED6-AF7B-302B5064A401}" name="Term Accession Number [hour] (#2; #h; #tUO:0000032; #u)"/>
-    <tableColumn id="9" xr3:uid="{8E4917AE-EF0F-4DF8-BFD2-BFF146FD82EC}" name="Factor [time]" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{BD204463-13F5-4B27-8D77-6411E54A0161}" name="Term Source REF [time] (#h; #tPATO:0000165)"/>
-    <tableColumn id="11" xr3:uid="{54079477-BBF2-47FA-A32F-D327F369CAB6}" name="Term Accession Number [time] (#h; #tPATO:0000165)"/>
-    <tableColumn id="12" xr3:uid="{898BAECA-1EB1-469E-8422-9998781D9728}" name="Unit [hour] (#h; #tUO:0000032; #u)"/>
-    <tableColumn id="13" xr3:uid="{79D7E23E-7DE5-42BF-B438-0B3C66A48687}" name="Term Source REF [hour] (#h; #tUO:0000032; #u)"/>
-    <tableColumn id="14" xr3:uid="{9440AB8D-FFDB-44A6-A041-2C27D8ADE0E9}" name="Term Accession Number [hour] (#h; #tUO:0000032; #u)"/>
+    <tableColumn id="28" xr3:uid="{AAD82B6E-D534-4041-A45F-3B4DE315F57C}" name="Term Source REF (NCIT:C16965)"/>
+    <tableColumn id="29" xr3:uid="{0832B850-0B29-42BE-8818-06D777F94D14}" name="Term Accession Number (NCIT:C16965)"/>
+    <tableColumn id="21" xr3:uid="{E885C835-8F07-49F7-8754-56F33C22EDA3}" name="Parameter [temperature#2]"/>
+    <tableColumn id="24" xr3:uid="{BBE00F76-3C9D-4912-9F00-79E953EFA580}" name="Unit (#2)"/>
+    <tableColumn id="25" xr3:uid="{4AFB1872-5F15-4214-A991-0EDD612D46C7}" name="Term Source REF (NCRO:0000029#2)"/>
+    <tableColumn id="26" xr3:uid="{3E7927AE-9C04-424E-9AF3-067EB934366D}" name="Term Accession Number (NCRO:0000029#2)"/>
+    <tableColumn id="15" xr3:uid="{0C97A092-0954-4712-ADFD-111FF359043F}" name="Parameter [time#3]"/>
+    <tableColumn id="18" xr3:uid="{48EE2CE6-DE17-43D9-931B-B49173F44C6D}" name="Unit (#3)"/>
+    <tableColumn id="19" xr3:uid="{6792D8C2-693B-4BC9-883A-51034FF96CE1}" name="Term Source REF (EFO:0000721#3)"/>
+    <tableColumn id="20" xr3:uid="{44AC5DB4-A15D-4ED6-AF7B-302B5064A401}" name="Term Accession Number (EFO:0000721#3)"/>
+    <tableColumn id="9" xr3:uid="{8E4917AE-EF0F-4DF8-BFD2-BFF146FD82EC}" name="Factor [time#4]" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{898BAECA-1EB1-469E-8422-9998781D9728}" name="Unit (#4)"/>
+    <tableColumn id="13" xr3:uid="{79D7E23E-7DE5-42BF-B438-0B3C66A48687}" name="Term Source REF (PATO:0000165#4)"/>
+    <tableColumn id="14" xr3:uid="{9440AB8D-FFDB-44A6-A041-2C27D8ADE0E9}" name="Term Accession Number (PATO:0000165#4)"/>
     <tableColumn id="2" xr3:uid="{A722F381-C4D5-4813-8976-3E815F9241E9}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -957,22 +933,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{80A48FB8-710D-4363-841A-CC6D7C1D1113}" name="annotationTable1" displayName="annotationTable1" ref="A2:N5" totalsRowShown="0">
-  <autoFilter ref="A2:N5" xr:uid="{FA614308-1200-4D41-8A17-2079200B2A5B}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{80A48FB8-710D-4363-841A-CC6D7C1D1113}" name="annotationTable1" displayName="annotationTable1" ref="A2:J5" totalsRowShown="0">
+  <autoFilter ref="A2:J5" xr:uid="{FA614308-1200-4D41-8A17-2079200B2A5B}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{C3F3E1B6-F85B-442A-9247-3F942C56FD58}" name="Source Name"/>
     <tableColumn id="9" xr3:uid="{949FFFA0-2A06-41CA-B58F-666F1213A2EC}" name="Characteristics [leaf size]"/>
-    <tableColumn id="10" xr3:uid="{5E002055-1412-42A0-BD52-7A94CEBF514E}" name="Term Source REF [leaf size] (#h; #tTO:0002637)"/>
-    <tableColumn id="11" xr3:uid="{01A64850-4546-4CCB-BD54-79C76F670459}" name="Term Accession Number [leaf size] (#h; #tTO:0002637)"/>
-    <tableColumn id="12" xr3:uid="{F4AB9CBF-7398-4BD4-B1D6-8BB53B14F67D}" name="Unit [square centimeter] (#h; #tUO:0000081; #u)"/>
-    <tableColumn id="13" xr3:uid="{F67602D1-FD31-4533-9F49-C5F6CF5239FF}" name="Term Source REF [square centimeter] (#h; #tUO:0000081; #u)"/>
-    <tableColumn id="14" xr3:uid="{BEC1E2C0-5194-42AE-B918-4F9222A4A0A9}" name="Term Accession Number [square centimeter] (#h; #tUO:0000081; #u)"/>
-    <tableColumn id="3" xr3:uid="{0632D05E-BACA-4B16-A8E9-BD1173DF5DE8}" name="Parameter [temperature unit]"/>
-    <tableColumn id="4" xr3:uid="{D01223E3-615D-4573-93FF-EB13FF8DF39B}" name="Term Source REF [temperature unit] (#h; #tUO:0000005)"/>
-    <tableColumn id="5" xr3:uid="{0C287CA6-2B4B-4878-AE2F-06CB480F22DC}" name="Term Accession Number [temperature unit] (#h; #tUO:0000005)"/>
-    <tableColumn id="6" xr3:uid="{DD1631B1-A456-4824-84CE-C5F90AD3B25A}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)"/>
-    <tableColumn id="7" xr3:uid="{5E0F81DB-9B29-474C-BCD1-840502C31A7C}" name="Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)"/>
-    <tableColumn id="8" xr3:uid="{7B3D90DC-0243-4149-B670-62221B996E73}" name="Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)"/>
+    <tableColumn id="12" xr3:uid="{F4AB9CBF-7398-4BD4-B1D6-8BB53B14F67D}" name="Unit"/>
+    <tableColumn id="13" xr3:uid="{F67602D1-FD31-4533-9F49-C5F6CF5239FF}" name="Term Source REF (TO:0002637)"/>
+    <tableColumn id="14" xr3:uid="{BEC1E2C0-5194-42AE-B918-4F9222A4A0A9}" name="Term Accession Number (TO:0002637)"/>
+    <tableColumn id="3" xr3:uid="{0632D05E-BACA-4B16-A8E9-BD1173DF5DE8}" name="Parameter [temperature unit#2]"/>
+    <tableColumn id="6" xr3:uid="{DD1631B1-A456-4824-84CE-C5F90AD3B25A}" name="Unit (#2)"/>
+    <tableColumn id="7" xr3:uid="{5E0F81DB-9B29-474C-BCD1-840502C31A7C}" name="Term Source REF (UO:0000005#2)"/>
+    <tableColumn id="8" xr3:uid="{7B3D90DC-0243-4149-B670-62221B996E73}" name="Term Accession Number (UO:0000005#2)" dataCellStyle="Hyperlink"/>
     <tableColumn id="2" xr3:uid="{BD54D798-70BF-4C8B-8C20-089B8BF190B0}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1294,56 +1266,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5703125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="43.28515625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="54.42578125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="61.5703125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.28515625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="54.42578125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="51.7109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="58.85546875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="45.5703125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="56.5703125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="63.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="42.5703125" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="49.7109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="37.28515625" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="48.28515625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="55.42578125" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="44" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="51.140625" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="34.140625" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="45.28515625" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="52.28515625" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.3046875" customWidth="1"/>
+    <col min="4" max="4" width="54.3828125" customWidth="1"/>
+    <col min="5" max="5" width="61.53515625" customWidth="1"/>
+    <col min="6" max="6" width="23.69140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.3046875" customWidth="1"/>
+    <col min="8" max="8" width="54.3828125" customWidth="1"/>
+    <col min="9" max="9" width="26.15234375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.53515625" customWidth="1"/>
+    <col min="11" max="11" width="56.53515625" customWidth="1"/>
+    <col min="12" max="12" width="63.69140625" customWidth="1"/>
+    <col min="13" max="13" width="18.69140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="37.3046875" customWidth="1"/>
+    <col min="15" max="15" width="48.3046875" customWidth="1"/>
+    <col min="16" max="16" width="55.3828125" customWidth="1"/>
+    <col min="17" max="17" width="14.69140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.15234375" customWidth="1"/>
+    <col min="19" max="19" width="45.3046875" customWidth="1"/>
+    <col min="20" max="20" width="52.3046875" customWidth="1"/>
+    <col min="21" max="21" width="42.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="9" t="s">
-        <v>78</v>
-      </c>
+      <c r="F1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
@@ -1352,21 +1316,13 @@
       <c r="N1" s="9"/>
       <c r="O1" s="9"/>
       <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="2"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="2"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1374,302 +1330,298 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R2" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" t="s">
+        <v>73</v>
+      </c>
+      <c r="T2" t="s">
         <v>74</v>
       </c>
-      <c r="I2" t="s">
-        <v>75</v>
-      </c>
-      <c r="J2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L2" t="s">
-        <v>68</v>
-      </c>
-      <c r="M2" t="s">
-        <v>69</v>
-      </c>
-      <c r="N2" t="s">
-        <v>70</v>
-      </c>
-      <c r="O2" t="s">
-        <v>71</v>
-      </c>
-      <c r="P2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>61</v>
-      </c>
-      <c r="R2" t="s">
-        <v>62</v>
-      </c>
-      <c r="S2" t="s">
-        <v>63</v>
-      </c>
-      <c r="T2" t="s">
-        <v>64</v>
-      </c>
       <c r="U2" t="s">
-        <v>65</v>
-      </c>
-      <c r="V2" t="s">
-        <v>66</v>
-      </c>
-      <c r="W2" t="s">
-        <v>31</v>
-      </c>
-      <c r="X2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3">
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
+        <v>44</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="3">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" t="s">
         <v>42</v>
       </c>
-      <c r="J3" t="s">
-        <v>76</v>
-      </c>
-      <c r="K3" s="3">
-        <v>37</v>
+      <c r="L3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="5">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="Q3" s="5">
-        <v>1</v>
-      </c>
-      <c r="W3" s="5">
         <v>10</v>
       </c>
-      <c r="X3" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3">
         <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" t="s">
-        <v>53</v>
+        <v>44</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="3">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" t="s">
         <v>42</v>
       </c>
-      <c r="J4" t="s">
-        <v>76</v>
-      </c>
-      <c r="K4" s="3">
+      <c r="L4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>4</v>
+      </c>
+      <c r="R4" t="s">
+        <v>45</v>
+      </c>
+      <c r="S4" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4" t="s">
         <v>37</v>
       </c>
-      <c r="Q4" s="5">
-        <v>1</v>
-      </c>
-      <c r="W4" s="5">
-        <v>4</v>
-      </c>
-      <c r="X4" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3">
         <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" t="s">
-        <v>53</v>
+        <v>44</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="G5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="3">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" t="s">
         <v>42</v>
       </c>
-      <c r="J5" t="s">
-        <v>76</v>
-      </c>
-      <c r="K5" s="3">
-        <v>37</v>
+      <c r="L5" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="5">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="Q5" s="5">
-        <v>1</v>
-      </c>
-      <c r="W5" s="5">
         <v>4</v>
       </c>
-      <c r="X5" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>49</v>
+      <c r="R5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" t="s">
+        <v>42</v>
+      </c>
+      <c r="T5" t="s">
+        <v>46</v>
+      </c>
+      <c r="U5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H1:V1"/>
+    <mergeCell ref="F1:P1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="L3" r:id="rId1" xr:uid="{2F83F38F-BB38-4E70-A555-3431EF854FAE}"/>
+    <hyperlink ref="P4" r:id="rId2" xr:uid="{060C3392-7473-4091-8630-5D642ADB7FEF}"/>
+    <hyperlink ref="P3" r:id="rId3" xr:uid="{08BAFB56-463F-4835-A6C5-B9ABD16A58D7}"/>
+    <hyperlink ref="P5" r:id="rId4" xr:uid="{D90EDBA4-DED5-422A-B738-52BABE2680BC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085B5FC8-A73A-4ACF-93D2-5463F7E84D95}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="46.7109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="57.85546875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="64.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="53.5703125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="60.5703125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="43.28515625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="54.42578125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="61.5703125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.69140625" customWidth="1"/>
+    <col min="4" max="4" width="57.84375" customWidth="1"/>
+    <col min="5" max="5" width="64.84375" customWidth="1"/>
+    <col min="6" max="6" width="30.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.3046875" customWidth="1"/>
+    <col min="8" max="8" width="54.3828125" customWidth="1"/>
+    <col min="9" max="9" width="61.53515625" customWidth="1"/>
+    <col min="10" max="10" width="15.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1679,103 +1631,151 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G2" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B3" s="8">
         <v>10</v>
       </c>
-      <c r="H3" s="3">
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="3">
         <v>37</v>
       </c>
-      <c r="N3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B4" s="8">
         <v>10</v>
       </c>
-      <c r="H4" s="3">
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="3">
         <v>37</v>
       </c>
-      <c r="N4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B5" s="8">
         <v>10</v>
       </c>
-      <c r="H5" s="3">
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="3">
         <v>37</v>
       </c>
-      <c r="N5" t="s">
-        <v>81</v>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{B253A599-C7F0-4BC5-8A23-1DBBE23D477B}"/>
+    <hyperlink ref="E4:E5" r:id="rId2" display="http://purl.obolibrary.org/obo/UO_0000081" xr:uid="{6A5AF3B1-7C2B-443B-A909-2EEE1B80166A}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{A422676D-BA5A-443A-844D-6F84B6C96A9C}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{9651701F-4FC2-403F-8F99-D0252A127F77}"/>
+    <hyperlink ref="I3" r:id="rId5" xr:uid="{B49FAFE8-D549-49DF-ABCC-0B2610E40900}"/>
+    <hyperlink ref="I4:I5" r:id="rId6" display="http://purl.obolibrary.org/obo/UO_0000081" xr:uid="{7ED22EC9-2B39-4C65-A57B-9C8E0266950B}"/>
+    <hyperlink ref="I4" r:id="rId7" xr:uid="{5810BAE9-4FFD-473B-9ACE-08EC295538A7}"/>
+    <hyperlink ref="I5" r:id="rId8" xr:uid="{2EF2E8B4-4E0F-4DF4-AAE2-E991DAC58A41}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1788,17 +1788,17 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="51.140625" customWidth="1"/>
+    <col min="1" max="1" width="51.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1822,31 +1822,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1854,50 +1854,50 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1937,39 +1937,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add study xlsx file io
</commit_message>
<xml_diff>
--- a/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTestFile.xlsx
+++ b/tests/ISADotNet.Tests/ISADotNet.XLSX/TestFiles/AssayTestFile.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLWei\source\repos\ISADotNet\tests\ISADotNet.Tests\ISADotNet.XLSX\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B8E0A3-198A-416D-9EBC-877CF8DBFB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B1AD37-44D2-4749-BE4C-4E12871BCDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="4230" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16629" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GreatAssay" sheetId="2" r:id="rId1"/>
     <sheet name="SecondAssay" sheetId="1" r:id="rId2"/>
-    <sheet name="Investigation" sheetId="3" r:id="rId3"/>
+    <sheet name="Assay" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1230,7 +1230,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="" visibility="1" width="350" row="3">
+  <wetp:taskpane dockstate="" visibility="1" width="613" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1250,7 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFD2A7E-D0F0-408B-A989-C09EBA475D3B}">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1709,7 +1709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F015C6-6FFA-4E23-9A41-FE00E4BAA0A3}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C25" sqref="C25:E25"/>
     </sheetView>
   </sheetViews>

</xml_diff>